<commit_message>
almost done - tests to perform
</commit_message>
<xml_diff>
--- a/src/demos/zdemo_excel15#1.w3mi.data.xlsx
+++ b/src/demos/zdemo_excel15#1.w3mi.data.xlsx
@@ -397,7 +397,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="B1:C15"/>
+  <dimension ref="B2:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" zoomScaleSheetLayoutView="100" workbookViewId="0" showGridLines="1" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -408,28 +408,28 @@
     <col min="2" max="2" width="1.1000000000000000E+01" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="0.0000000000000000E+00">
+    <row r="1" spans="1:3">
       <c r=""/>
     </row>
-    <row r="2" spans="1:3" ht="0.0000000000000000E+00">
+    <row r="2" spans="1:3">
       <c r="B2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="0.0000000000000000E+00">
+    <row r="3" spans="1:3">
       <c r="B3" s="2">
-        <v>44533</v>
+        <v>44534</v>
       </c>
       <c r="C3" s="3">
-        <v>0.5422569444444445</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="0.0000000000000000E+00">
+        <v>0.4749884259259259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="B4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="0.0000000000000000E+00">
+    <row r="6" spans="1:3">
       <c r="B6" t="s">
         <v>20</v>
       </c>
@@ -437,7 +437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="0.0000000000000000E+00">
+    <row r="7" spans="1:3">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -445,7 +445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="0.0000000000000000E+00">
+    <row r="8" spans="1:3">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -453,7 +453,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="0.0000000000000000E+00">
+    <row r="9" spans="1:3">
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -461,7 +461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="0.0000000000000000E+00">
+    <row r="10" spans="1:3">
       <c r="B10" t="s">
         <v>19</v>
       </c>
@@ -469,7 +469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="0.0000000000000000E+00">
+    <row r="11" spans="1:3">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -477,7 +477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="0.0000000000000000E+00">
+    <row r="12" spans="1:3">
       <c r="B12" t="s">
         <v>14</v>
       </c>
@@ -485,7 +485,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="0.0000000000000000E+00">
+    <row r="13" spans="1:3">
       <c r="B13" t="s">
         <v>15</v>
       </c>
@@ -493,7 +493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="0.0000000000000000E+00">
+    <row r="14" spans="1:3">
       <c r="B14" t="s">
         <v>17</v>
       </c>
@@ -501,7 +501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="0.0000000000000000E+00">
+    <row r="15" spans="1:3">
       <c r="B15" t="s">
         <v>21</v>
       </c>
@@ -510,6 +510,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup/>
 </worksheet>

</xml_diff>